<commit_message>
merge intervals end of first approach
</commit_message>
<xml_diff>
--- a/56. Merge Intervals/Whiteboards/Solution.xlsx
+++ b/56. Merge Intervals/Whiteboards/Solution.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\56. Merge Intervals\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A42D85-A705-4C8E-ADD1-6F64C7103B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B2D042-8D1D-4139-8E57-0A277287DE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,6 +35,17 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>5,5</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -45,7 +57,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -64,8 +76,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -73,30 +91,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -104,6 +104,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -420,265 +426,1071 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="H14:AR62"/>
+  <dimension ref="H6:AR80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AD60" sqref="AD60"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA75" sqref="AA75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="4.7109375" style="2"/>
+    <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="14" spans="9:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="9:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="9:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="12:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="12:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="12:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N19" s="1"/>
+    <row r="6" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>3</v>
+      </c>
+      <c r="L6" s="1">
+        <v>4</v>
+      </c>
+      <c r="M6" s="1">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1">
+        <v>6</v>
+      </c>
+      <c r="O6" s="1">
+        <v>7</v>
+      </c>
+      <c r="P6" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>9</v>
+      </c>
+      <c r="R6" s="1">
+        <v>10</v>
+      </c>
+      <c r="S6" s="1">
+        <v>11</v>
+      </c>
+      <c r="T6" s="1">
+        <v>12</v>
+      </c>
+      <c r="U6" s="1">
+        <v>13</v>
+      </c>
+      <c r="V6" s="1">
+        <v>14</v>
+      </c>
+      <c r="W6" s="1">
+        <v>15</v>
+      </c>
+      <c r="X6" s="1">
+        <v>16</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>17</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>18</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>19</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>20</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>21</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>22</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>23</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>24</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>25</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>26</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>27</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>28</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>29</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>30</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>31</v>
+      </c>
+      <c r="AN6" s="1">
+        <v>32</v>
+      </c>
+      <c r="AO6" s="1">
+        <v>33</v>
+      </c>
+      <c r="AP6" s="1">
+        <v>34</v>
+      </c>
+      <c r="AQ6" s="1">
+        <v>35</v>
+      </c>
+      <c r="AR6" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
+      <c r="N9" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T10" s="2">
+        <v>12</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE11" s="2">
+        <v>23</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ12" s="2">
+        <v>28</v>
+      </c>
+      <c r="AL12" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN13" s="2">
+        <v>32</v>
+      </c>
+      <c r="AO13" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AO14" s="2">
+        <v>33</v>
+      </c>
+      <c r="AP14" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P15" s="2">
+        <v>8</v>
+      </c>
+      <c r="U15" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE16" s="2">
+        <v>23</v>
+      </c>
+      <c r="AH16" s="3">
+        <v>26</v>
+      </c>
+      <c r="AK16" s="2">
+        <v>29</v>
+      </c>
+      <c r="AL16" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="2">
+        <v>1</v>
+      </c>
+      <c r="J21" s="2">
+        <v>2</v>
+      </c>
+      <c r="K21" s="3">
+        <v>3</v>
+      </c>
+      <c r="N21" s="3">
+        <v>6</v>
+      </c>
+      <c r="P21" s="2">
+        <v>8</v>
+      </c>
+      <c r="T21" s="2">
+        <v>12</v>
+      </c>
+      <c r="U21" s="3">
+        <v>13</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>19</v>
+      </c>
+      <c r="AE21" s="2">
+        <v>23</v>
+      </c>
+      <c r="AG21" s="3">
+        <v>25</v>
+      </c>
+      <c r="AH21" s="3">
+        <v>26</v>
+      </c>
+      <c r="AJ21" s="2">
+        <v>28</v>
+      </c>
+      <c r="AK21" s="2">
+        <v>29</v>
+      </c>
+      <c r="AL21" s="3">
+        <v>30</v>
+      </c>
+      <c r="AN21" s="2">
+        <v>32</v>
+      </c>
+      <c r="AO21" s="3">
+        <v>33</v>
+      </c>
+      <c r="AP21" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE22" s="2">
+        <v>23</v>
+      </c>
+      <c r="AL22" s="3">
+        <v>30</v>
+      </c>
+      <c r="AO22" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AJ23" s="2"/>
+      <c r="AK23" s="2"/>
+      <c r="AL23" s="2"/>
+      <c r="AN23" s="2"/>
+      <c r="AO23" s="2"/>
+      <c r="AP23" s="2"/>
+    </row>
+    <row r="25" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1">
+        <v>2</v>
+      </c>
+      <c r="K25" s="1">
+        <v>3</v>
+      </c>
+      <c r="L25" s="1">
+        <v>4</v>
+      </c>
+      <c r="M25" s="1">
+        <v>5</v>
+      </c>
+      <c r="N25" s="1">
+        <v>6</v>
+      </c>
+      <c r="O25" s="1">
+        <v>7</v>
+      </c>
+      <c r="P25" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>9</v>
+      </c>
+      <c r="R25" s="1">
+        <v>10</v>
+      </c>
+      <c r="S25" s="1">
+        <v>11</v>
+      </c>
+      <c r="T25" s="1">
+        <v>12</v>
+      </c>
+      <c r="U25" s="1">
+        <v>13</v>
+      </c>
+      <c r="V25" s="1">
+        <v>14</v>
+      </c>
+      <c r="W25" s="1">
+        <v>15</v>
+      </c>
+      <c r="X25" s="1">
+        <v>16</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>17</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>18</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>19</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>20</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>21</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>22</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>23</v>
+      </c>
+      <c r="AF25" s="1">
+        <v>24</v>
+      </c>
+      <c r="AG25" s="1">
+        <v>25</v>
+      </c>
+      <c r="AH25" s="1">
+        <v>26</v>
+      </c>
+      <c r="AI25" s="1">
+        <v>27</v>
+      </c>
+      <c r="AJ25" s="1">
+        <v>28</v>
+      </c>
+      <c r="AK25" s="1">
+        <v>29</v>
+      </c>
+      <c r="AL25" s="1">
+        <v>30</v>
+      </c>
+      <c r="AM25" s="1">
+        <v>31</v>
+      </c>
+      <c r="AN25" s="1">
+        <v>32</v>
+      </c>
+      <c r="AO25" s="1">
+        <v>33</v>
+      </c>
+      <c r="AP25" s="1">
+        <v>34</v>
+      </c>
+      <c r="AQ25" s="1">
+        <v>35</v>
+      </c>
+      <c r="AR25" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="1">
+        <v>2</v>
+      </c>
+      <c r="K26" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M27" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J28" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="1">
+        <v>3</v>
+      </c>
+      <c r="L29" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K30" s="1">
+        <v>3</v>
+      </c>
+      <c r="L30" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="2">
+        <v>2</v>
+      </c>
+      <c r="K32" s="3">
+        <v>3</v>
+      </c>
+      <c r="L32" s="3">
+        <v>4</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K33" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <v>1</v>
+      </c>
+      <c r="J36" s="1">
+        <v>2</v>
+      </c>
+      <c r="K36" s="1">
+        <v>3</v>
+      </c>
+      <c r="L36" s="1">
+        <v>4</v>
+      </c>
+      <c r="M36" s="1">
+        <v>5</v>
+      </c>
+      <c r="N36" s="1">
+        <v>6</v>
+      </c>
+      <c r="O36" s="1">
+        <v>7</v>
+      </c>
+      <c r="P36" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>9</v>
+      </c>
+      <c r="R36" s="1">
+        <v>10</v>
+      </c>
+      <c r="S36" s="1">
+        <v>11</v>
+      </c>
+      <c r="T36" s="1">
+        <v>12</v>
+      </c>
+      <c r="U36" s="1">
+        <v>13</v>
+      </c>
+      <c r="V36" s="1">
+        <v>14</v>
+      </c>
+      <c r="W36" s="1">
+        <v>15</v>
+      </c>
+      <c r="X36" s="1">
+        <v>16</v>
+      </c>
+      <c r="Y36" s="1">
+        <v>17</v>
+      </c>
+      <c r="Z36" s="1">
+        <v>18</v>
+      </c>
+      <c r="AA36" s="1">
+        <v>19</v>
+      </c>
+      <c r="AB36" s="1">
+        <v>20</v>
+      </c>
+      <c r="AC36" s="1">
+        <v>21</v>
+      </c>
+      <c r="AD36" s="1">
+        <v>22</v>
+      </c>
+      <c r="AE36" s="1">
+        <v>23</v>
+      </c>
+      <c r="AF36" s="1">
+        <v>24</v>
+      </c>
+      <c r="AG36" s="1">
+        <v>25</v>
+      </c>
+      <c r="AH36" s="1">
+        <v>26</v>
+      </c>
+      <c r="AI36" s="1">
+        <v>27</v>
+      </c>
+      <c r="AJ36" s="1">
+        <v>28</v>
+      </c>
+      <c r="AK36" s="1">
+        <v>29</v>
+      </c>
+      <c r="AL36" s="1">
+        <v>30</v>
+      </c>
+      <c r="AM36" s="1">
+        <v>31</v>
+      </c>
+      <c r="AN36" s="1">
+        <v>32</v>
+      </c>
+      <c r="AO36" s="1">
+        <v>33</v>
+      </c>
+      <c r="AP36" s="1">
+        <v>34</v>
+      </c>
+      <c r="AQ36" s="1">
+        <v>35</v>
+      </c>
+      <c r="AR36" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="2">
+        <v>0</v>
+      </c>
+      <c r="J38" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="2">
+        <v>1</v>
+      </c>
+      <c r="L39" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K40" s="2">
+        <v>3</v>
+      </c>
+      <c r="M40" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="2">
+        <v>0</v>
+      </c>
+      <c r="I43" s="2">
+        <v>1</v>
+      </c>
+      <c r="J43" s="3">
+        <v>2</v>
+      </c>
+      <c r="K43" s="2">
+        <v>3</v>
+      </c>
+      <c r="L43" s="3">
+        <v>4</v>
+      </c>
+      <c r="M43" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="47" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H47" s="2">
+      <c r="I47" s="2">
+        <v>1</v>
+      </c>
+      <c r="L47" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M48" s="2">
+        <v>5</v>
+      </c>
+      <c r="N48" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="2">
+        <v>1</v>
+      </c>
+      <c r="L50" s="3">
+        <v>4</v>
+      </c>
+      <c r="M50" s="2">
+        <v>5</v>
+      </c>
+      <c r="N50" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H54" s="1">
         <v>0</v>
       </c>
-      <c r="I47" s="2">
-        <v>1</v>
-      </c>
-      <c r="J47" s="2">
-        <v>2</v>
-      </c>
-      <c r="K47" s="2">
-        <v>3</v>
-      </c>
-      <c r="L47" s="2">
-        <v>4</v>
-      </c>
-      <c r="M47" s="2">
+      <c r="I54" s="1">
+        <v>1</v>
+      </c>
+      <c r="J54" s="1">
+        <v>2</v>
+      </c>
+      <c r="K54" s="1">
+        <v>3</v>
+      </c>
+      <c r="L54" s="1">
+        <v>4</v>
+      </c>
+      <c r="M54" s="1">
         <v>5</v>
       </c>
-      <c r="N47" s="2">
+      <c r="N54" s="1">
         <v>6</v>
       </c>
-      <c r="O47" s="2">
+      <c r="O54" s="1">
         <v>7</v>
       </c>
-      <c r="P47" s="2">
+      <c r="P54" s="1">
         <v>8</v>
       </c>
-      <c r="Q47" s="2">
+      <c r="Q54" s="1">
         <v>9</v>
       </c>
-      <c r="R47" s="2">
+      <c r="R54" s="1">
         <v>10</v>
       </c>
-      <c r="S47" s="2">
+      <c r="S54" s="1">
         <v>11</v>
       </c>
-      <c r="T47" s="2">
+      <c r="T54" s="1">
         <v>12</v>
       </c>
-      <c r="U47" s="2">
+      <c r="U54" s="1">
         <v>13</v>
       </c>
-      <c r="V47" s="2">
+      <c r="V54" s="1">
         <v>14</v>
       </c>
-      <c r="W47" s="2">
+      <c r="W54" s="1">
         <v>15</v>
       </c>
-      <c r="X47" s="2">
+      <c r="X54" s="1">
         <v>16</v>
       </c>
-      <c r="Y47" s="2">
+      <c r="Y54" s="1">
         <v>17</v>
       </c>
-      <c r="Z47" s="2">
+      <c r="Z54" s="1">
         <v>18</v>
       </c>
-      <c r="AA47" s="2">
+      <c r="AA54" s="1">
         <v>19</v>
       </c>
-      <c r="AB47" s="2">
+      <c r="AB54" s="1">
         <v>20</v>
       </c>
-      <c r="AC47" s="2">
+      <c r="AC54" s="1">
         <v>21</v>
       </c>
-      <c r="AD47" s="2">
+      <c r="AD54" s="1">
         <v>22</v>
       </c>
-      <c r="AE47" s="2">
+      <c r="AE54" s="1">
         <v>23</v>
       </c>
-      <c r="AF47" s="2">
+      <c r="AF54" s="1">
         <v>24</v>
       </c>
-      <c r="AG47" s="2">
+      <c r="AG54" s="1">
         <v>25</v>
       </c>
-      <c r="AH47" s="2">
+      <c r="AH54" s="1">
         <v>26</v>
       </c>
-      <c r="AI47" s="2">
+      <c r="AI54" s="1">
         <v>27</v>
       </c>
-      <c r="AJ47" s="2">
+      <c r="AJ54" s="1">
         <v>28</v>
       </c>
-      <c r="AK47" s="2">
+      <c r="AK54" s="1">
         <v>29</v>
       </c>
-      <c r="AL47" s="2">
+      <c r="AL54" s="1">
         <v>30</v>
       </c>
-      <c r="AM47" s="2">
+      <c r="AM54" s="1">
         <v>31</v>
       </c>
-      <c r="AN47" s="2">
+      <c r="AN54" s="1">
         <v>32</v>
       </c>
-      <c r="AO47" s="2">
+      <c r="AO54" s="1">
         <v>33</v>
       </c>
-      <c r="AP47" s="2">
+      <c r="AP54" s="1">
         <v>34</v>
       </c>
-      <c r="AQ47" s="2">
+      <c r="AQ54" s="1">
         <v>35</v>
       </c>
-      <c r="AR47" s="2">
+      <c r="AR54" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I48" s="3">
-        <v>1</v>
-      </c>
-      <c r="K48" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="9:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J50" s="3">
-        <v>2</v>
-      </c>
-      <c r="N50" s="4">
+    <row r="55" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J55" s="2">
+        <v>2</v>
+      </c>
+      <c r="K55" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J56" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K57" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I58" s="2">
+        <v>1</v>
+      </c>
+      <c r="K58" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M59" s="2">
+        <v>5</v>
+      </c>
+      <c r="O59" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J60" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L61" s="2">
+        <v>4</v>
+      </c>
+      <c r="N61" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="9:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T51" s="3">
+    <row r="63" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I63" s="2">
+        <v>1</v>
+      </c>
+      <c r="J63" s="2">
+        <v>2</v>
+      </c>
+      <c r="K63" s="3">
+        <v>3</v>
+      </c>
+      <c r="L63" s="2">
+        <v>4</v>
+      </c>
+      <c r="M63" s="2">
+        <v>5</v>
+      </c>
+      <c r="N63" s="3">
+        <v>6</v>
+      </c>
+      <c r="O63" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J64" s="4">
+        <v>22</v>
+      </c>
+      <c r="K64" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J65" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H68" s="1">
+        <v>0</v>
+      </c>
+      <c r="I68" s="1">
+        <v>1</v>
+      </c>
+      <c r="J68" s="1">
+        <v>2</v>
+      </c>
+      <c r="K68" s="1">
+        <v>3</v>
+      </c>
+      <c r="L68" s="1">
+        <v>4</v>
+      </c>
+      <c r="M68" s="1">
+        <v>5</v>
+      </c>
+      <c r="N68" s="1">
+        <v>6</v>
+      </c>
+      <c r="O68" s="1">
+        <v>7</v>
+      </c>
+      <c r="P68" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q68" s="1">
+        <v>9</v>
+      </c>
+      <c r="R68" s="1">
+        <v>10</v>
+      </c>
+      <c r="S68" s="1">
+        <v>11</v>
+      </c>
+      <c r="T68" s="1">
         <v>12</v>
       </c>
-      <c r="AA51" s="4">
+      <c r="U68" s="1">
+        <v>13</v>
+      </c>
+      <c r="V68" s="1">
+        <v>14</v>
+      </c>
+      <c r="W68" s="1">
+        <v>15</v>
+      </c>
+      <c r="X68" s="1">
+        <v>16</v>
+      </c>
+      <c r="Y68" s="1">
+        <v>17</v>
+      </c>
+      <c r="Z68" s="1">
+        <v>18</v>
+      </c>
+      <c r="AA68" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="52" spans="9:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AE52" s="3">
+      <c r="AB68" s="1">
+        <v>20</v>
+      </c>
+      <c r="AC68" s="1">
+        <v>21</v>
+      </c>
+      <c r="AD68" s="1">
+        <v>22</v>
+      </c>
+      <c r="AE68" s="1">
         <v>23</v>
       </c>
-      <c r="AG52" s="4">
+      <c r="AF68" s="1">
+        <v>24</v>
+      </c>
+      <c r="AG68" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="53" spans="9:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AJ53" s="3">
+      <c r="AH68" s="1">
+        <v>26</v>
+      </c>
+      <c r="AI68" s="1">
+        <v>27</v>
+      </c>
+      <c r="AJ68" s="1">
         <v>28</v>
       </c>
-      <c r="AL53" s="4">
+      <c r="AK68" s="1">
+        <v>29</v>
+      </c>
+      <c r="AL68" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="54" spans="9:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AN54" s="3">
+      <c r="AM68" s="1">
+        <v>31</v>
+      </c>
+      <c r="AN68" s="1">
         <v>32</v>
       </c>
-      <c r="AO54" s="4">
+      <c r="AO68" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="55" spans="9:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AO55" s="3">
+      <c r="AP68" s="1">
+        <v>34</v>
+      </c>
+      <c r="AQ68" s="1">
+        <v>35</v>
+      </c>
+      <c r="AR68" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I69" s="2">
+        <v>1</v>
+      </c>
+      <c r="K69" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H70" s="2">
+        <v>0</v>
+      </c>
+      <c r="J70" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J71" s="2">
+        <v>2</v>
+      </c>
+      <c r="K71" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L72" s="2">
+        <v>4</v>
+      </c>
+      <c r="N72" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L73" s="2">
+        <v>4</v>
+      </c>
+      <c r="M73" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M74" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H75" s="2">
+        <v>0</v>
+      </c>
+      <c r="J75" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K76" s="4">
         <v>33</v>
       </c>
-      <c r="AP55" s="4">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="56" spans="9:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P56" s="3">
-        <v>8</v>
-      </c>
-      <c r="U56" s="4">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="57" spans="9:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AE57" s="3">
-        <v>23</v>
-      </c>
-      <c r="AH57" s="4">
-        <v>26</v>
-      </c>
-      <c r="AK57" s="3">
-        <v>29</v>
-      </c>
-      <c r="AL57" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="62" spans="9:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I62" s="3">
-        <v>1</v>
-      </c>
-      <c r="J62" s="3">
-        <v>2</v>
-      </c>
-      <c r="K62" s="4">
-        <v>3</v>
-      </c>
-      <c r="N62" s="4">
+    </row>
+    <row r="78" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H78" s="2">
+        <v>0</v>
+      </c>
+      <c r="I78" s="2">
+        <v>1</v>
+      </c>
+      <c r="J78" s="3">
+        <v>2</v>
+      </c>
+      <c r="K78" s="3">
+        <v>3</v>
+      </c>
+      <c r="L78" s="2">
+        <v>4</v>
+      </c>
+      <c r="M78" s="3">
+        <v>5</v>
+      </c>
+      <c r="N78" s="3">
         <v>6</v>
       </c>
-      <c r="P62" s="3">
-        <v>8</v>
-      </c>
-      <c r="T62" s="3">
-        <v>12</v>
-      </c>
-      <c r="U62" s="4">
-        <v>13</v>
-      </c>
-      <c r="AA62" s="4">
-        <v>19</v>
+    </row>
+    <row r="79" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H79" s="2">
+        <v>0</v>
+      </c>
+      <c r="J79" s="3">
+        <v>2</v>
+      </c>
+      <c r="K79" s="3">
+        <v>3</v>
+      </c>
+      <c r="L79" s="2">
+        <v>4</v>
+      </c>
+      <c r="M79" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="8:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J80" s="2">
+        <v>2</v>
+      </c>
+      <c r="K80" s="4">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#56 saved excel notes
</commit_message>
<xml_diff>
--- a/56. Merge Intervals/Whiteboards/Solution.xlsx
+++ b/56. Merge Intervals/Whiteboards/Solution.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\56. Merge Intervals\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B2D042-8D1D-4139-8E57-0A277287DE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA242110-6503-4CCE-89FC-3C0D0B6F3721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,22 +36,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
   <si>
     <t>2,2</t>
   </si>
   <si>
     <t>5,5</t>
   </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>p1[0]</t>
+  </si>
+  <si>
+    <t>p1[1]</t>
+  </si>
+  <si>
+    <t>p2[0]</t>
+  </si>
+  <si>
+    <t>p2[1]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -111,6 +138,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
   <dimension ref="H6:AR80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AA75" sqref="AA75"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1497,4 +1539,161 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E03F3B-6217-4F8B-B7C9-F1728ED89378}">
+  <dimension ref="K9:AE32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="4.7109375" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="11:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K9" s="6">
+        <v>1</v>
+      </c>
+      <c r="L9" s="6">
+        <v>2</v>
+      </c>
+      <c r="M9" s="6">
+        <v>3</v>
+      </c>
+      <c r="N9" s="6">
+        <v>4</v>
+      </c>
+      <c r="O9" s="6">
+        <v>5</v>
+      </c>
+      <c r="P9" s="6">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>7</v>
+      </c>
+      <c r="R9" s="6">
+        <v>8</v>
+      </c>
+      <c r="S9" s="6">
+        <v>9</v>
+      </c>
+      <c r="T9" s="6">
+        <v>10</v>
+      </c>
+      <c r="U9" s="6">
+        <v>11</v>
+      </c>
+      <c r="V9" s="6">
+        <v>12</v>
+      </c>
+      <c r="W9" s="6">
+        <v>13</v>
+      </c>
+      <c r="X9" s="6">
+        <v>14</v>
+      </c>
+      <c r="Y9" s="6">
+        <v>15</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>16</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>17</v>
+      </c>
+      <c r="AB9" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="11:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="11:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="11:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="S15" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="11:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE16" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="11:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K19" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="S19" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="11:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="11:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="S23" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="11:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P24" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="11:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M32" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>